<commit_message>
registros sin coincidencias, archivos con errores
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -561,13 +561,13 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>850</v>
+        <v>870</v>
       </c>
       <c r="H2" t="n">
         <v>800</v>
       </c>
       <c r="I2" t="n">
-        <v>900</v>
+        <v>940</v>
       </c>
       <c r="J2" t="n">
         <v>0.33</v>
@@ -576,19 +576,19 @@
         <v>1500</v>
       </c>
       <c r="L2" t="n">
-        <v>680</v>
+        <v>655</v>
       </c>
       <c r="M2" t="n">
-        <v>600</v>
+        <v>560</v>
       </c>
       <c r="N2" t="n">
-        <v>680</v>
+        <v>655</v>
       </c>
       <c r="O2" t="n">
-        <v>680</v>
+        <v>655</v>
       </c>
       <c r="P2" t="n">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="Q2" t="n">
         <v>54.54545454545455</v>
@@ -602,7 +602,7 @@
         </is>
       </c>
       <c r="T2" t="n">
-        <v>0.35</v>
+        <v>0.32</v>
       </c>
     </row>
     <row r="3">
@@ -631,11 +631,13 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>850</v>
-      </c>
-      <c r="H3" t="inlineStr"/>
+        <v>860</v>
+      </c>
+      <c r="H3" t="n">
+        <v>800</v>
+      </c>
       <c r="I3" t="n">
-        <v>920</v>
+        <v>900</v>
       </c>
       <c r="J3" t="n">
         <v>0.38</v>
@@ -644,15 +646,19 @@
         <v>1500</v>
       </c>
       <c r="L3" t="n">
-        <v>660</v>
-      </c>
-      <c r="M3" t="inlineStr"/>
-      <c r="N3" t="inlineStr"/>
+        <v>490</v>
+      </c>
+      <c r="M3" t="n">
+        <v>390</v>
+      </c>
+      <c r="N3" t="n">
+        <v>490</v>
+      </c>
       <c r="O3" t="n">
-        <v>660</v>
+        <v>490</v>
       </c>
       <c r="P3" t="n">
-        <v>58</v>
+        <v>100</v>
       </c>
       <c r="Q3" t="n">
         <v>62.06896551724138</v>
@@ -665,7 +671,9 @@
           <t>ok</t>
         </is>
       </c>
-      <c r="T3" t="inlineStr"/>
+      <c r="T3" t="n">
+        <v>0.31</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -757,9 +765,11 @@
       <c r="G5" t="n">
         <v>870</v>
       </c>
-      <c r="H5" t="inlineStr"/>
+      <c r="H5" t="n">
+        <v>800</v>
+      </c>
       <c r="I5" t="n">
-        <v>930</v>
+        <v>920</v>
       </c>
       <c r="J5" t="n">
         <v>0.31</v>
@@ -768,12 +778,16 @@
         <v>1500</v>
       </c>
       <c r="L5" t="n">
-        <v>510</v>
-      </c>
-      <c r="M5" t="inlineStr"/>
-      <c r="N5" t="inlineStr"/>
+        <v>515</v>
+      </c>
+      <c r="M5" t="n">
+        <v>430</v>
+      </c>
+      <c r="N5" t="n">
+        <v>515</v>
+      </c>
       <c r="O5" t="n">
-        <v>510</v>
+        <v>515</v>
       </c>
       <c r="P5" t="n">
         <v>70</v>
@@ -789,7 +803,9 @@
           <t>ok</t>
         </is>
       </c>
-      <c r="T5" t="inlineStr"/>
+      <c r="T5" t="n">
+        <v>0.31</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -964,19 +980,19 @@
         <v>1500</v>
       </c>
       <c r="L8" t="n">
-        <v>702</v>
+        <v>555</v>
       </c>
       <c r="M8" t="n">
-        <v>625</v>
+        <v>450</v>
       </c>
       <c r="N8" t="n">
-        <v>702</v>
+        <v>555</v>
       </c>
       <c r="O8" t="n">
-        <v>702</v>
+        <v>555</v>
       </c>
       <c r="P8" t="n">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="Q8" t="n">
         <v>36</v>
@@ -1064,10 +1080,8 @@
       <c r="B10" t="n">
         <v>5.5</v>
       </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>0,476</t>
-        </is>
+      <c r="C10" t="n">
+        <v>0.476</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -1083,11 +1097,13 @@
         </is>
       </c>
       <c r="G10" t="n">
-        <v>850</v>
-      </c>
-      <c r="H10" t="inlineStr"/>
+        <v>860</v>
+      </c>
+      <c r="H10" t="n">
+        <v>800</v>
+      </c>
       <c r="I10" t="n">
-        <v>900</v>
+        <v>920</v>
       </c>
       <c r="J10" t="n">
         <v>0.2</v>
@@ -1098,8 +1114,12 @@
       <c r="L10" t="n">
         <v>530</v>
       </c>
-      <c r="M10" t="inlineStr"/>
-      <c r="N10" t="inlineStr"/>
+      <c r="M10" t="n">
+        <v>450</v>
+      </c>
+      <c r="N10" t="n">
+        <v>530</v>
+      </c>
       <c r="O10" t="n">
         <v>530</v>
       </c>
@@ -1117,7 +1137,9 @@
           <t>ok</t>
         </is>
       </c>
-      <c r="T10" t="inlineStr"/>
+      <c r="T10" t="n">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1145,28 +1167,34 @@
         </is>
       </c>
       <c r="G11" t="n">
-        <v>870</v>
-      </c>
-      <c r="H11" t="inlineStr"/>
+        <v>860</v>
+      </c>
+      <c r="H11" t="n">
+        <v>800</v>
+      </c>
       <c r="I11" t="n">
-        <v>890</v>
+        <v>930</v>
       </c>
       <c r="J11" t="n">
         <v>0.27</v>
       </c>
       <c r="K11" t="n">
-        <v>1450</v>
+        <v>1500</v>
       </c>
       <c r="L11" t="n">
-        <v>655</v>
-      </c>
-      <c r="M11" t="inlineStr"/>
-      <c r="N11" t="inlineStr"/>
+        <v>650</v>
+      </c>
+      <c r="M11" t="n">
+        <v>560</v>
+      </c>
+      <c r="N11" t="n">
+        <v>650</v>
+      </c>
       <c r="O11" t="n">
-        <v>655</v>
+        <v>650</v>
       </c>
       <c r="P11" t="n">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="Q11" t="n">
         <v>55.38461538461539</v>
@@ -1179,7 +1207,9 @@
           <t>ok</t>
         </is>
       </c>
-      <c r="T11" t="inlineStr"/>
+      <c r="T11" t="n">
+        <v>0.26</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1207,9 +1237,11 @@
         </is>
       </c>
       <c r="G12" t="n">
-        <v>860</v>
-      </c>
-      <c r="H12" t="inlineStr"/>
+        <v>870</v>
+      </c>
+      <c r="H12" t="n">
+        <v>800</v>
+      </c>
       <c r="I12" t="n">
         <v>920</v>
       </c>
@@ -1220,15 +1252,19 @@
         <v>1500</v>
       </c>
       <c r="L12" t="n">
-        <v>673</v>
-      </c>
-      <c r="M12" t="inlineStr"/>
-      <c r="N12" t="inlineStr"/>
+        <v>490</v>
+      </c>
+      <c r="M12" t="n">
+        <v>390</v>
+      </c>
+      <c r="N12" t="n">
+        <v>490</v>
+      </c>
       <c r="O12" t="n">
-        <v>673</v>
+        <v>490</v>
       </c>
       <c r="P12" t="n">
-        <v>95</v>
+        <v>140</v>
       </c>
       <c r="Q12" t="n">
         <v>37.89473684210526</v>
@@ -1241,7 +1277,9 @@
           <t>ok</t>
         </is>
       </c>
-      <c r="T12" t="inlineStr"/>
+      <c r="T12" t="n">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1331,9 +1369,11 @@
         </is>
       </c>
       <c r="G14" t="n">
-        <v>860</v>
-      </c>
-      <c r="H14" t="inlineStr"/>
+        <v>870</v>
+      </c>
+      <c r="H14" t="n">
+        <v>800</v>
+      </c>
       <c r="I14" t="n">
         <v>920</v>
       </c>
@@ -1344,15 +1384,19 @@
         <v>1500</v>
       </c>
       <c r="L14" t="n">
-        <v>715</v>
-      </c>
-      <c r="M14" t="inlineStr"/>
-      <c r="N14" t="inlineStr"/>
+        <v>490</v>
+      </c>
+      <c r="M14" t="n">
+        <v>390</v>
+      </c>
+      <c r="N14" t="n">
+        <v>490</v>
+      </c>
       <c r="O14" t="n">
-        <v>715</v>
+        <v>490</v>
       </c>
       <c r="P14" t="n">
-        <v>64</v>
+        <v>140</v>
       </c>
       <c r="Q14" t="n">
         <v>56.25</v>
@@ -1365,7 +1409,9 @@
           <t>ok</t>
         </is>
       </c>
-      <c r="T14" t="inlineStr"/>
+      <c r="T14" t="n">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1395,7 +1441,9 @@
       <c r="G15" t="n">
         <v>860</v>
       </c>
-      <c r="H15" t="inlineStr"/>
+      <c r="H15" t="n">
+        <v>800</v>
+      </c>
       <c r="I15" t="n">
         <v>920</v>
       </c>
@@ -1406,15 +1454,19 @@
         <v>1500</v>
       </c>
       <c r="L15" t="n">
-        <v>650</v>
-      </c>
-      <c r="M15" t="inlineStr"/>
-      <c r="N15" t="inlineStr"/>
+        <v>525</v>
+      </c>
+      <c r="M15" t="n">
+        <v>430</v>
+      </c>
+      <c r="N15" t="n">
+        <v>525</v>
+      </c>
       <c r="O15" t="n">
-        <v>650</v>
+        <v>525</v>
       </c>
       <c r="P15" t="n">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="Q15" t="n">
         <v>52.17391304347826</v>
@@ -1427,7 +1479,9 @@
           <t>ok</t>
         </is>
       </c>
-      <c r="T15" t="inlineStr"/>
+      <c r="T15" t="n">
+        <v>26</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1517,28 +1571,34 @@
         </is>
       </c>
       <c r="G17" t="n">
-        <v>830</v>
-      </c>
-      <c r="H17" t="inlineStr"/>
+        <v>870</v>
+      </c>
+      <c r="H17" t="n">
+        <v>800</v>
+      </c>
       <c r="I17" t="n">
-        <v>900</v>
+        <v>920</v>
       </c>
       <c r="J17" t="n">
         <v>0.23</v>
       </c>
       <c r="K17" t="n">
-        <v>1400</v>
+        <v>1500</v>
       </c>
       <c r="L17" t="n">
-        <v>555</v>
-      </c>
-      <c r="M17" t="inlineStr"/>
-      <c r="N17" t="inlineStr"/>
+        <v>490</v>
+      </c>
+      <c r="M17" t="n">
+        <v>390</v>
+      </c>
+      <c r="N17" t="n">
+        <v>490</v>
+      </c>
       <c r="O17" t="n">
-        <v>555</v>
+        <v>490</v>
       </c>
       <c r="P17" t="n">
-        <v>95</v>
+        <v>140</v>
       </c>
       <c r="Q17" t="n">
         <v>37.89473684210526</v>
@@ -1551,7 +1611,9 @@
           <t>ok</t>
         </is>
       </c>
-      <c r="T17" t="inlineStr"/>
+      <c r="T17" t="n">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1581,7 +1643,9 @@
       <c r="G18" t="n">
         <v>870</v>
       </c>
-      <c r="H18" t="inlineStr"/>
+      <c r="H18" t="n">
+        <v>800</v>
+      </c>
       <c r="I18" t="n">
         <v>920</v>
       </c>
@@ -1594,13 +1658,17 @@
       <c r="L18" t="n">
         <v>490</v>
       </c>
-      <c r="M18" t="inlineStr"/>
-      <c r="N18" t="inlineStr"/>
+      <c r="M18" t="n">
+        <v>390</v>
+      </c>
+      <c r="N18" t="n">
+        <v>490</v>
+      </c>
       <c r="O18" t="n">
         <v>490</v>
       </c>
       <c r="P18" t="n">
-        <v>88</v>
+        <v>140</v>
       </c>
       <c r="Q18" t="n">
         <v>40.90909090909091</v>
@@ -1613,7 +1681,9 @@
           <t>ok</t>
         </is>
       </c>
-      <c r="T18" t="inlineStr"/>
+      <c r="T18" t="n">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1827,28 +1897,34 @@
         </is>
       </c>
       <c r="G22" t="n">
-        <v>850</v>
-      </c>
-      <c r="H22" t="inlineStr"/>
+        <v>860</v>
+      </c>
+      <c r="H22" t="n">
+        <v>800</v>
+      </c>
       <c r="I22" t="n">
-        <v>910</v>
+        <v>900</v>
       </c>
       <c r="J22" t="n">
         <v>0.21</v>
       </c>
       <c r="K22" t="n">
-        <v>1400</v>
+        <v>1500</v>
       </c>
       <c r="L22" t="n">
-        <v>670</v>
-      </c>
-      <c r="M22" t="inlineStr"/>
-      <c r="N22" t="inlineStr"/>
+        <v>525</v>
+      </c>
+      <c r="M22" t="n">
+        <v>430</v>
+      </c>
+      <c r="N22" t="n">
+        <v>525</v>
+      </c>
       <c r="O22" t="n">
-        <v>670</v>
+        <v>525</v>
       </c>
       <c r="P22" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="Q22" t="n">
         <v>36</v>
@@ -1861,7 +1937,9 @@
           <t>ok</t>
         </is>
       </c>
-      <c r="T22" t="inlineStr"/>
+      <c r="T22" t="n">
+        <v>23</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1889,28 +1967,34 @@
         </is>
       </c>
       <c r="G23" t="n">
-        <v>850</v>
-      </c>
-      <c r="H23" t="inlineStr"/>
+        <v>860</v>
+      </c>
+      <c r="H23" t="n">
+        <v>800</v>
+      </c>
       <c r="I23" t="n">
-        <v>890</v>
+        <v>900</v>
       </c>
       <c r="J23" t="n">
         <v>0.26</v>
       </c>
       <c r="K23" t="n">
-        <v>1600</v>
+        <v>1500</v>
       </c>
       <c r="L23" t="n">
-        <v>645</v>
-      </c>
-      <c r="M23" t="inlineStr"/>
-      <c r="N23" t="inlineStr"/>
+        <v>525</v>
+      </c>
+      <c r="M23" t="n">
+        <v>430</v>
+      </c>
+      <c r="N23" t="n">
+        <v>525</v>
+      </c>
       <c r="O23" t="n">
-        <v>645</v>
+        <v>525</v>
       </c>
       <c r="P23" t="n">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="Q23" t="n">
         <v>50</v>
@@ -1923,7 +2007,9 @@
           <t>ok</t>
         </is>
       </c>
-      <c r="T23" t="inlineStr"/>
+      <c r="T23" t="n">
+        <v>23</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1951,11 +2037,13 @@
         </is>
       </c>
       <c r="G24" t="n">
-        <v>860</v>
-      </c>
-      <c r="H24" t="inlineStr"/>
+        <v>870</v>
+      </c>
+      <c r="H24" t="n">
+        <v>800</v>
+      </c>
       <c r="I24" t="n">
-        <v>900</v>
+        <v>920</v>
       </c>
       <c r="J24" t="n">
         <v>0.26</v>
@@ -1964,15 +2052,19 @@
         <v>1500</v>
       </c>
       <c r="L24" t="n">
-        <v>710</v>
-      </c>
-      <c r="M24" t="inlineStr"/>
-      <c r="N24" t="inlineStr"/>
+        <v>490</v>
+      </c>
+      <c r="M24" t="n">
+        <v>390</v>
+      </c>
+      <c r="N24" t="n">
+        <v>490</v>
+      </c>
       <c r="O24" t="n">
-        <v>710</v>
+        <v>490</v>
       </c>
       <c r="P24" t="n">
-        <v>72</v>
+        <v>140</v>
       </c>
       <c r="Q24" t="n">
         <v>50</v>
@@ -1985,7 +2077,9 @@
           <t>ok</t>
         </is>
       </c>
-      <c r="T24" t="inlineStr"/>
+      <c r="T24" t="n">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -2013,11 +2107,13 @@
         </is>
       </c>
       <c r="G25" t="n">
-        <v>860</v>
-      </c>
-      <c r="H25" t="inlineStr"/>
+        <v>870</v>
+      </c>
+      <c r="H25" t="n">
+        <v>800</v>
+      </c>
       <c r="I25" t="n">
-        <v>890</v>
+        <v>920</v>
       </c>
       <c r="J25" t="n">
         <v>0.25</v>
@@ -2026,15 +2122,19 @@
         <v>1500</v>
       </c>
       <c r="L25" t="n">
-        <v>640</v>
-      </c>
-      <c r="M25" t="inlineStr"/>
-      <c r="N25" t="inlineStr"/>
+        <v>490</v>
+      </c>
+      <c r="M25" t="n">
+        <v>390</v>
+      </c>
+      <c r="N25" t="n">
+        <v>490</v>
+      </c>
       <c r="O25" t="n">
-        <v>640</v>
+        <v>490</v>
       </c>
       <c r="P25" t="n">
-        <v>75</v>
+        <v>140</v>
       </c>
       <c r="Q25" t="n">
         <v>48</v>
@@ -2047,7 +2147,9 @@
           <t>ok</t>
         </is>
       </c>
-      <c r="T25" t="inlineStr"/>
+      <c r="T25" t="n">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -2137,28 +2239,34 @@
         </is>
       </c>
       <c r="G27" t="n">
-        <v>860</v>
-      </c>
-      <c r="H27" t="inlineStr"/>
+        <v>880</v>
+      </c>
+      <c r="H27" t="n">
+        <v>780</v>
+      </c>
       <c r="I27" t="n">
-        <v>900</v>
+        <v>910</v>
       </c>
       <c r="J27" t="n">
         <v>0.22</v>
       </c>
       <c r="K27" t="n">
-        <v>1450</v>
+        <v>1500</v>
       </c>
       <c r="L27" t="n">
-        <v>720</v>
-      </c>
-      <c r="M27" t="inlineStr"/>
-      <c r="N27" t="inlineStr"/>
+        <v>700</v>
+      </c>
+      <c r="M27" t="n">
+        <v>660</v>
+      </c>
+      <c r="N27" t="n">
+        <v>700</v>
+      </c>
       <c r="O27" t="n">
-        <v>720</v>
+        <v>700</v>
       </c>
       <c r="P27" t="n">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="Q27" t="n">
         <v>34.28571428571428</v>
@@ -2171,7 +2279,9 @@
           <t>ok</t>
         </is>
       </c>
-      <c r="T27" t="inlineStr"/>
+      <c r="T27" t="n">
+        <v>21</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -2201,7 +2311,9 @@
       <c r="G28" t="n">
         <v>860</v>
       </c>
-      <c r="H28" t="inlineStr"/>
+      <c r="H28" t="n">
+        <v>800</v>
+      </c>
       <c r="I28" t="n">
         <v>920</v>
       </c>
@@ -2214,8 +2326,12 @@
       <c r="L28" t="n">
         <v>525</v>
       </c>
-      <c r="M28" t="inlineStr"/>
-      <c r="N28" t="inlineStr"/>
+      <c r="M28" t="n">
+        <v>430</v>
+      </c>
+      <c r="N28" t="n">
+        <v>525</v>
+      </c>
       <c r="O28" t="n">
         <v>525</v>
       </c>
@@ -2233,7 +2349,9 @@
           <t>ok</t>
         </is>
       </c>
-      <c r="T28" t="inlineStr"/>
+      <c r="T28" t="n">
+        <v>26</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -2263,7 +2381,9 @@
       <c r="G29" t="n">
         <v>860</v>
       </c>
-      <c r="H29" t="inlineStr"/>
+      <c r="H29" t="n">
+        <v>800</v>
+      </c>
       <c r="I29" t="n">
         <v>920</v>
       </c>
@@ -2276,8 +2396,12 @@
       <c r="L29" t="n">
         <v>525</v>
       </c>
-      <c r="M29" t="inlineStr"/>
-      <c r="N29" t="inlineStr"/>
+      <c r="M29" t="n">
+        <v>430</v>
+      </c>
+      <c r="N29" t="n">
+        <v>525</v>
+      </c>
       <c r="O29" t="n">
         <v>525</v>
       </c>
@@ -2295,7 +2419,9 @@
           <t>ok</t>
         </is>
       </c>
-      <c r="T29" t="inlineStr"/>
+      <c r="T29" t="n">
+        <v>26</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -2325,7 +2451,9 @@
       <c r="G30" t="n">
         <v>860</v>
       </c>
-      <c r="H30" t="inlineStr"/>
+      <c r="H30" t="n">
+        <v>800</v>
+      </c>
       <c r="I30" t="n">
         <v>920</v>
       </c>
@@ -2336,15 +2464,19 @@
         <v>1500</v>
       </c>
       <c r="L30" t="n">
-        <v>560</v>
-      </c>
-      <c r="M30" t="inlineStr"/>
-      <c r="N30" t="inlineStr"/>
+        <v>525</v>
+      </c>
+      <c r="M30" t="n">
+        <v>430</v>
+      </c>
+      <c r="N30" t="n">
+        <v>525</v>
+      </c>
       <c r="O30" t="n">
-        <v>560</v>
+        <v>525</v>
       </c>
       <c r="P30" t="n">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="Q30" t="n">
         <v>43.37349397590361</v>
@@ -2357,7 +2489,9 @@
           <t>ok</t>
         </is>
       </c>
-      <c r="T30" t="inlineStr"/>
+      <c r="T30" t="n">
+        <v>26</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -2387,7 +2521,9 @@
       <c r="G31" t="n">
         <v>860</v>
       </c>
-      <c r="H31" t="inlineStr"/>
+      <c r="H31" t="n">
+        <v>800</v>
+      </c>
       <c r="I31" t="n">
         <v>920</v>
       </c>
@@ -2400,8 +2536,12 @@
       <c r="L31" t="n">
         <v>525</v>
       </c>
-      <c r="M31" t="inlineStr"/>
-      <c r="N31" t="inlineStr"/>
+      <c r="M31" t="n">
+        <v>430</v>
+      </c>
+      <c r="N31" t="n">
+        <v>525</v>
+      </c>
       <c r="O31" t="n">
         <v>525</v>
       </c>
@@ -2419,7 +2559,9 @@
           <t>ok</t>
         </is>
       </c>
-      <c r="T31" t="inlineStr"/>
+      <c r="T31" t="n">
+        <v>26</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -2449,26 +2591,32 @@
       <c r="G32" t="n">
         <v>860</v>
       </c>
-      <c r="H32" t="inlineStr"/>
+      <c r="H32" t="n">
+        <v>800</v>
+      </c>
       <c r="I32" t="n">
-        <v>890</v>
+        <v>900</v>
       </c>
       <c r="J32" t="n">
         <v>0.23</v>
       </c>
       <c r="K32" t="n">
-        <v>1450</v>
+        <v>1500</v>
       </c>
       <c r="L32" t="n">
-        <v>490</v>
-      </c>
-      <c r="M32" t="inlineStr"/>
-      <c r="N32" t="inlineStr"/>
+        <v>525</v>
+      </c>
+      <c r="M32" t="n">
+        <v>430</v>
+      </c>
+      <c r="N32" t="n">
+        <v>525</v>
+      </c>
       <c r="O32" t="n">
-        <v>490</v>
+        <v>525</v>
       </c>
       <c r="P32" t="n">
-        <v>140</v>
+        <v>80</v>
       </c>
       <c r="Q32" t="n">
         <v>25.71428571428572</v>
@@ -2481,7 +2629,9 @@
           <t>ok</t>
         </is>
       </c>
-      <c r="T32" t="inlineStr"/>
+      <c r="T32" t="n">
+        <v>23</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -2881,11 +3031,13 @@
         </is>
       </c>
       <c r="G39" t="n">
-        <v>860</v>
-      </c>
-      <c r="H39" t="inlineStr"/>
+        <v>880</v>
+      </c>
+      <c r="H39" t="n">
+        <v>800</v>
+      </c>
       <c r="I39" t="n">
-        <v>890</v>
+        <v>915</v>
       </c>
       <c r="J39" t="n">
         <v>0.22</v>
@@ -2894,15 +3046,19 @@
         <v>1500</v>
       </c>
       <c r="L39" t="n">
-        <v>675</v>
-      </c>
-      <c r="M39" t="inlineStr"/>
-      <c r="N39" t="inlineStr"/>
+        <v>520</v>
+      </c>
+      <c r="M39" t="n">
+        <v>450</v>
+      </c>
+      <c r="N39" t="n">
+        <v>520</v>
+      </c>
       <c r="O39" t="n">
-        <v>675</v>
+        <v>520</v>
       </c>
       <c r="P39" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="Q39" t="n">
         <v>36</v>
@@ -2915,7 +3071,9 @@
           <t>ok</t>
         </is>
       </c>
-      <c r="T39" t="inlineStr"/>
+      <c r="T39" t="n">
+        <v>0.21</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -2943,11 +3101,13 @@
         </is>
       </c>
       <c r="G40" t="n">
-        <v>870</v>
-      </c>
-      <c r="H40" t="inlineStr"/>
+        <v>880</v>
+      </c>
+      <c r="H40" t="n">
+        <v>800</v>
+      </c>
       <c r="I40" t="n">
-        <v>910</v>
+        <v>915</v>
       </c>
       <c r="J40" t="n">
         <v>0.24</v>
@@ -2956,15 +3116,19 @@
         <v>1500</v>
       </c>
       <c r="L40" t="n">
-        <v>640</v>
-      </c>
-      <c r="M40" t="inlineStr"/>
-      <c r="N40" t="inlineStr"/>
+        <v>520</v>
+      </c>
+      <c r="M40" t="n">
+        <v>450</v>
+      </c>
+      <c r="N40" t="n">
+        <v>520</v>
+      </c>
       <c r="O40" t="n">
-        <v>640</v>
+        <v>520</v>
       </c>
       <c r="P40" t="n">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="Q40" t="n">
         <v>45</v>
@@ -2977,7 +3141,9 @@
           <t>ok</t>
         </is>
       </c>
-      <c r="T40" t="inlineStr"/>
+      <c r="T40" t="n">
+        <v>0.21</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -3687,11 +3853,13 @@
         </is>
       </c>
       <c r="G52" t="n">
-        <v>860</v>
-      </c>
-      <c r="H52" t="inlineStr"/>
+        <v>880</v>
+      </c>
+      <c r="H52" t="n">
+        <v>800</v>
+      </c>
       <c r="I52" t="n">
-        <v>890</v>
+        <v>915</v>
       </c>
       <c r="J52" t="n">
         <v>0.2</v>
@@ -3700,15 +3868,19 @@
         <v>1500</v>
       </c>
       <c r="L52" t="n">
-        <v>535</v>
-      </c>
-      <c r="M52" t="inlineStr"/>
-      <c r="N52" t="inlineStr"/>
+        <v>520</v>
+      </c>
+      <c r="M52" t="n">
+        <v>450</v>
+      </c>
+      <c r="N52" t="n">
+        <v>520</v>
+      </c>
       <c r="O52" t="n">
-        <v>535</v>
+        <v>520</v>
       </c>
       <c r="P52" t="n">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="Q52" t="n">
         <v>40</v>
@@ -3721,7 +3893,9 @@
           <t>ok</t>
         </is>
       </c>
-      <c r="T52" t="inlineStr"/>
+      <c r="T52" t="n">
+        <v>0.21</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -3813,23 +3987,29 @@
       <c r="G54" t="n">
         <v>860</v>
       </c>
-      <c r="H54" t="inlineStr"/>
+      <c r="H54" t="n">
+        <v>800</v>
+      </c>
       <c r="I54" t="n">
-        <v>940</v>
+        <v>900</v>
       </c>
       <c r="J54" t="n">
         <v>0.2</v>
       </c>
       <c r="K54" t="n">
-        <v>1500</v>
+        <v>1400</v>
       </c>
       <c r="L54" t="n">
-        <v>635</v>
-      </c>
-      <c r="M54" t="inlineStr"/>
-      <c r="N54" t="inlineStr"/>
+        <v>525</v>
+      </c>
+      <c r="M54" t="n">
+        <v>460</v>
+      </c>
+      <c r="N54" t="n">
+        <v>525</v>
+      </c>
       <c r="O54" t="n">
-        <v>653</v>
+        <v>525</v>
       </c>
       <c r="P54" t="n">
         <v>85</v>
@@ -3845,7 +4025,9 @@
           <t>ok</t>
         </is>
       </c>
-      <c r="T54" t="inlineStr"/>
+      <c r="T54" t="n">
+        <v>0.21</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -3875,7 +4057,9 @@
       <c r="G55" t="n">
         <v>860</v>
       </c>
-      <c r="H55" t="inlineStr"/>
+      <c r="H55" t="n">
+        <v>800</v>
+      </c>
       <c r="I55" t="n">
         <v>900</v>
       </c>
@@ -3886,12 +4070,16 @@
         <v>1400</v>
       </c>
       <c r="L55" t="n">
-        <v>520</v>
-      </c>
-      <c r="M55" t="inlineStr"/>
-      <c r="N55" t="inlineStr"/>
+        <v>525</v>
+      </c>
+      <c r="M55" t="n">
+        <v>460</v>
+      </c>
+      <c r="N55" t="n">
+        <v>525</v>
+      </c>
       <c r="O55" t="n">
-        <v>520</v>
+        <v>525</v>
       </c>
       <c r="P55" t="n">
         <v>85</v>
@@ -3907,7 +4095,9 @@
           <t>ok</t>
         </is>
       </c>
-      <c r="T55" t="inlineStr"/>
+      <c r="T55" t="n">
+        <v>0.21</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -3937,7 +4127,9 @@
       <c r="G56" t="n">
         <v>860</v>
       </c>
-      <c r="H56" t="inlineStr"/>
+      <c r="H56" t="n">
+        <v>800</v>
+      </c>
       <c r="I56" t="n">
         <v>900</v>
       </c>
@@ -3948,12 +4140,16 @@
         <v>1400</v>
       </c>
       <c r="L56" t="n">
-        <v>520</v>
-      </c>
-      <c r="M56" t="inlineStr"/>
-      <c r="N56" t="inlineStr"/>
+        <v>525</v>
+      </c>
+      <c r="M56" t="n">
+        <v>460</v>
+      </c>
+      <c r="N56" t="n">
+        <v>525</v>
+      </c>
       <c r="O56" t="n">
-        <v>520</v>
+        <v>525</v>
       </c>
       <c r="P56" t="n">
         <v>85</v>
@@ -3969,7 +4165,9 @@
           <t>ok</t>
         </is>
       </c>
-      <c r="T56" t="inlineStr"/>
+      <c r="T56" t="n">
+        <v>0.21</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -3999,7 +4197,9 @@
       <c r="G57" t="n">
         <v>870</v>
       </c>
-      <c r="H57" t="inlineStr"/>
+      <c r="H57" t="n">
+        <v>800</v>
+      </c>
       <c r="I57" t="n">
         <v>920</v>
       </c>
@@ -4010,12 +4210,16 @@
         <v>1400</v>
       </c>
       <c r="L57" t="n">
-        <v>525</v>
-      </c>
-      <c r="M57" t="inlineStr"/>
-      <c r="N57" t="inlineStr"/>
+        <v>530</v>
+      </c>
+      <c r="M57" t="n">
+        <v>450</v>
+      </c>
+      <c r="N57" t="n">
+        <v>530</v>
+      </c>
       <c r="O57" t="n">
-        <v>525</v>
+        <v>530</v>
       </c>
       <c r="P57" t="n">
         <v>85</v>
@@ -4031,7 +4235,9 @@
           <t>ok</t>
         </is>
       </c>
-      <c r="T57" t="inlineStr"/>
+      <c r="T57" t="n">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -4061,7 +4267,9 @@
       <c r="G58" t="n">
         <v>870</v>
       </c>
-      <c r="H58" t="inlineStr"/>
+      <c r="H58" t="n">
+        <v>800</v>
+      </c>
       <c r="I58" t="n">
         <v>890</v>
       </c>
@@ -4074,8 +4282,12 @@
       <c r="L58" t="n">
         <v>655</v>
       </c>
-      <c r="M58" t="inlineStr"/>
-      <c r="N58" t="inlineStr"/>
+      <c r="M58" t="n">
+        <v>560</v>
+      </c>
+      <c r="N58" t="n">
+        <v>655</v>
+      </c>
       <c r="O58" t="n">
         <v>655</v>
       </c>
@@ -4093,7 +4305,9 @@
           <t>ok</t>
         </is>
       </c>
-      <c r="T58" t="inlineStr"/>
+      <c r="T58" t="n">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -4123,7 +4337,9 @@
       <c r="G59" t="n">
         <v>870</v>
       </c>
-      <c r="H59" t="inlineStr"/>
+      <c r="H59" t="n">
+        <v>800</v>
+      </c>
       <c r="I59" t="n">
         <v>920</v>
       </c>
@@ -4136,8 +4352,12 @@
       <c r="L59" t="n">
         <v>660</v>
       </c>
-      <c r="M59" t="inlineStr"/>
-      <c r="N59" t="inlineStr"/>
+      <c r="M59" t="n">
+        <v>560</v>
+      </c>
+      <c r="N59" t="n">
+        <v>660</v>
+      </c>
       <c r="O59" t="n">
         <v>660</v>
       </c>
@@ -4155,7 +4375,9 @@
           <t>ok</t>
         </is>
       </c>
-      <c r="T59" t="inlineStr"/>
+      <c r="T59" t="n">
+        <v>0.14</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -4183,9 +4405,11 @@
         </is>
       </c>
       <c r="G60" t="n">
-        <v>860</v>
-      </c>
-      <c r="H60" t="inlineStr"/>
+        <v>870</v>
+      </c>
+      <c r="H60" t="n">
+        <v>800</v>
+      </c>
       <c r="I60" t="n">
         <v>920</v>
       </c>
@@ -4193,18 +4417,22 @@
         <v>0.23</v>
       </c>
       <c r="K60" t="n">
-        <v>1500</v>
+        <v>1600</v>
       </c>
       <c r="L60" t="n">
         <v>660</v>
       </c>
-      <c r="M60" t="inlineStr"/>
-      <c r="N60" t="inlineStr"/>
+      <c r="M60" t="n">
+        <v>560</v>
+      </c>
+      <c r="N60" t="n">
+        <v>660</v>
+      </c>
       <c r="O60" t="n">
         <v>660</v>
       </c>
       <c r="P60" t="n">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="Q60" t="n">
         <v>42.85714285714285</v>
@@ -4217,7 +4445,9 @@
           <t>ok</t>
         </is>
       </c>
-      <c r="T60" t="inlineStr"/>
+      <c r="T60" t="n">
+        <v>0.19</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -4245,25 +4475,31 @@
         </is>
       </c>
       <c r="G61" t="n">
-        <v>850</v>
-      </c>
-      <c r="H61" t="inlineStr"/>
+        <v>870</v>
+      </c>
+      <c r="H61" t="n">
+        <v>800</v>
+      </c>
       <c r="I61" t="n">
-        <v>900</v>
+        <v>890</v>
       </c>
       <c r="J61" t="n">
         <v>0.18</v>
       </c>
       <c r="K61" t="n">
-        <v>1500</v>
+        <v>1600</v>
       </c>
       <c r="L61" t="n">
-        <v>685</v>
-      </c>
-      <c r="M61" t="inlineStr"/>
-      <c r="N61" t="inlineStr"/>
+        <v>700</v>
+      </c>
+      <c r="M61" t="n">
+        <v>600</v>
+      </c>
+      <c r="N61" t="n">
+        <v>700</v>
+      </c>
       <c r="O61" t="n">
-        <v>685</v>
+        <v>700</v>
       </c>
       <c r="P61" t="n">
         <v>111</v>
@@ -4279,7 +4515,9 @@
           <t>ok</t>
         </is>
       </c>
-      <c r="T61" t="inlineStr"/>
+      <c r="T61" t="n">
+        <v>0.18</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -4307,11 +4545,13 @@
         </is>
       </c>
       <c r="G62" t="n">
-        <v>870</v>
-      </c>
-      <c r="H62" t="inlineStr"/>
+        <v>880</v>
+      </c>
+      <c r="H62" t="n">
+        <v>800</v>
+      </c>
       <c r="I62" t="n">
-        <v>910</v>
+        <v>920</v>
       </c>
       <c r="J62" t="n">
         <v>0.23</v>
@@ -4320,15 +4560,19 @@
         <v>1500</v>
       </c>
       <c r="L62" t="n">
-        <v>705</v>
-      </c>
-      <c r="M62" t="inlineStr"/>
-      <c r="N62" t="inlineStr"/>
+        <v>540</v>
+      </c>
+      <c r="M62" t="n">
+        <v>500</v>
+      </c>
+      <c r="N62" t="n">
+        <v>540</v>
+      </c>
       <c r="O62" t="n">
-        <v>705</v>
+        <v>540</v>
       </c>
       <c r="P62" t="n">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="Q62" t="n">
         <v>38.70967741935484</v>
@@ -4341,7 +4585,9 @@
           <t>ok</t>
         </is>
       </c>
-      <c r="T62" t="inlineStr"/>
+      <c r="T62" t="n">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -4369,9 +4615,11 @@
         </is>
       </c>
       <c r="G63" t="n">
-        <v>880</v>
-      </c>
-      <c r="H63" t="inlineStr"/>
+        <v>860</v>
+      </c>
+      <c r="H63" t="n">
+        <v>800</v>
+      </c>
       <c r="I63" t="n">
         <v>910</v>
       </c>
@@ -4382,15 +4630,19 @@
         <v>1500</v>
       </c>
       <c r="L63" t="n">
-        <v>685</v>
-      </c>
-      <c r="M63" t="inlineStr"/>
-      <c r="N63" t="inlineStr"/>
+        <v>520</v>
+      </c>
+      <c r="M63" t="n">
+        <v>500</v>
+      </c>
+      <c r="N63" t="n">
+        <v>520</v>
+      </c>
       <c r="O63" t="n">
-        <v>685</v>
+        <v>520</v>
       </c>
       <c r="P63" t="n">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="Q63" t="n">
         <v>38.70967741935484</v>
@@ -4403,7 +4655,9 @@
           <t>ok</t>
         </is>
       </c>
-      <c r="T63" t="inlineStr"/>
+      <c r="T63" t="n">
+        <v>0.18</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -4431,9 +4685,11 @@
         </is>
       </c>
       <c r="G64" t="n">
-        <v>860</v>
-      </c>
-      <c r="H64" t="inlineStr"/>
+        <v>870</v>
+      </c>
+      <c r="H64" t="n">
+        <v>800</v>
+      </c>
       <c r="I64" t="n">
         <v>890</v>
       </c>
@@ -4446,8 +4702,12 @@
       <c r="L64" t="n">
         <v>700</v>
       </c>
-      <c r="M64" t="inlineStr"/>
-      <c r="N64" t="inlineStr"/>
+      <c r="M64" t="n">
+        <v>600</v>
+      </c>
+      <c r="N64" t="n">
+        <v>700</v>
+      </c>
       <c r="O64" t="n">
         <v>700</v>
       </c>
@@ -4465,7 +4725,9 @@
           <t>ok</t>
         </is>
       </c>
-      <c r="T64" t="inlineStr"/>
+      <c r="T64" t="n">
+        <v>0.18</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -4492,19 +4754,33 @@
           <t>SIDERCA</t>
         </is>
       </c>
-      <c r="G65" t="inlineStr"/>
-      <c r="H65" t="inlineStr"/>
-      <c r="I65" t="inlineStr"/>
+      <c r="G65" t="n">
+        <v>880</v>
+      </c>
+      <c r="H65" t="n">
+        <v>800</v>
+      </c>
+      <c r="I65" t="n">
+        <v>920</v>
+      </c>
       <c r="J65" t="inlineStr"/>
-      <c r="K65" t="inlineStr"/>
-      <c r="L65" t="inlineStr"/>
-      <c r="M65" t="inlineStr"/>
-      <c r="N65" t="inlineStr"/>
+      <c r="K65" t="n">
+        <v>1600</v>
+      </c>
+      <c r="L65" t="n">
+        <v>572</v>
+      </c>
+      <c r="M65" t="n">
+        <v>500</v>
+      </c>
+      <c r="N65" t="n">
+        <v>572</v>
+      </c>
       <c r="O65" t="n">
-        <v>555</v>
+        <v>572</v>
       </c>
       <c r="P65" t="n">
-        <v>97</v>
+        <v>110</v>
       </c>
       <c r="Q65" t="n">
         <v>37.11340206185567</v>
@@ -4517,7 +4793,9 @@
           <t>ok</t>
         </is>
       </c>
-      <c r="T65" t="inlineStr"/>
+      <c r="T65" t="n">
+        <v>0.18</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -4545,28 +4823,34 @@
         </is>
       </c>
       <c r="G66" t="n">
-        <v>880</v>
-      </c>
-      <c r="H66" t="inlineStr"/>
+        <v>860</v>
+      </c>
+      <c r="H66" t="n">
+        <v>800</v>
+      </c>
       <c r="I66" t="n">
-        <v>930</v>
+        <v>890</v>
       </c>
       <c r="J66" t="n">
         <v>0.2</v>
       </c>
       <c r="K66" t="n">
-        <v>1500</v>
+        <v>1600</v>
       </c>
       <c r="L66" t="n">
-        <v>670</v>
-      </c>
-      <c r="M66" t="inlineStr"/>
-      <c r="N66" t="inlineStr"/>
+        <v>545</v>
+      </c>
+      <c r="M66" t="n">
+        <v>460</v>
+      </c>
+      <c r="N66" t="n">
+        <v>545</v>
+      </c>
       <c r="O66" t="n">
-        <v>670</v>
+        <v>545</v>
       </c>
       <c r="P66" t="n">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="Q66" t="n">
         <v>31.30434782608696</v>
@@ -4579,7 +4863,9 @@
           <t>ok</t>
         </is>
       </c>
-      <c r="T66" t="inlineStr"/>
+      <c r="T66" t="n">
+        <v>0.18</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -4669,11 +4955,13 @@
         </is>
       </c>
       <c r="G68" t="n">
-        <v>870</v>
-      </c>
-      <c r="H68" t="inlineStr"/>
+        <v>860</v>
+      </c>
+      <c r="H68" t="n">
+        <v>800</v>
+      </c>
       <c r="I68" t="n">
-        <v>900</v>
+        <v>910</v>
       </c>
       <c r="J68" t="n">
         <v>0.18</v>
@@ -4684,8 +4972,12 @@
       <c r="L68" t="n">
         <v>520</v>
       </c>
-      <c r="M68" t="inlineStr"/>
-      <c r="N68" t="inlineStr"/>
+      <c r="M68" t="n">
+        <v>500</v>
+      </c>
+      <c r="N68" t="n">
+        <v>520</v>
+      </c>
       <c r="O68" t="n">
         <v>520</v>
       </c>
@@ -4703,7 +4995,9 @@
           <t>ok</t>
         </is>
       </c>
-      <c r="T68" t="inlineStr"/>
+      <c r="T68" t="n">
+        <v>0.18</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -4731,11 +5025,13 @@
         </is>
       </c>
       <c r="G69" t="n">
-        <v>880</v>
-      </c>
-      <c r="H69" t="inlineStr"/>
+        <v>860</v>
+      </c>
+      <c r="H69" t="n">
+        <v>800</v>
+      </c>
       <c r="I69" t="n">
-        <v>920</v>
+        <v>910</v>
       </c>
       <c r="J69" t="n">
         <v>0.2</v>
@@ -4744,15 +5040,19 @@
         <v>1500</v>
       </c>
       <c r="L69" t="n">
-        <v>655</v>
-      </c>
-      <c r="M69" t="inlineStr"/>
-      <c r="N69" t="inlineStr"/>
+        <v>520</v>
+      </c>
+      <c r="M69" t="n">
+        <v>500</v>
+      </c>
+      <c r="N69" t="n">
+        <v>520</v>
+      </c>
       <c r="O69" t="n">
-        <v>655</v>
+        <v>520</v>
       </c>
       <c r="P69" t="n">
-        <v>140</v>
+        <v>98</v>
       </c>
       <c r="Q69" t="n">
         <v>25.71428571428572</v>
@@ -4765,7 +5065,9 @@
           <t>ok</t>
         </is>
       </c>
-      <c r="T69" t="inlineStr"/>
+      <c r="T69" t="n">
+        <v>0.18</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -4793,28 +5095,34 @@
         </is>
       </c>
       <c r="G70" t="n">
-        <v>880</v>
-      </c>
-      <c r="H70" t="inlineStr"/>
+        <v>890</v>
+      </c>
+      <c r="H70" t="n">
+        <v>800</v>
+      </c>
       <c r="I70" t="n">
-        <v>920</v>
+        <v>900</v>
       </c>
       <c r="J70" t="n">
         <v>0.2</v>
       </c>
       <c r="K70" t="n">
-        <v>1500</v>
+        <v>1600</v>
       </c>
       <c r="L70" t="n">
-        <v>540</v>
-      </c>
-      <c r="M70" t="inlineStr"/>
-      <c r="N70" t="inlineStr"/>
+        <v>700</v>
+      </c>
+      <c r="M70" t="n">
+        <v>600</v>
+      </c>
+      <c r="N70" t="n">
+        <v>700</v>
+      </c>
       <c r="O70" t="n">
-        <v>540</v>
+        <v>700</v>
       </c>
       <c r="P70" t="n">
-        <v>98</v>
+        <v>120</v>
       </c>
       <c r="Q70" t="n">
         <v>36.73469387755102</v>
@@ -4827,7 +5135,9 @@
           <t>ok</t>
         </is>
       </c>
-      <c r="T70" t="inlineStr"/>
+      <c r="T70" t="n">
+        <v>0.17</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -4979,11 +5289,13 @@
         </is>
       </c>
       <c r="G73" t="n">
+        <v>860</v>
+      </c>
+      <c r="H73" t="n">
+        <v>800</v>
+      </c>
+      <c r="I73" t="n">
         <v>890</v>
-      </c>
-      <c r="H73" t="inlineStr"/>
-      <c r="I73" t="n">
-        <v>900</v>
       </c>
       <c r="J73" t="n">
         <v>0.17</v>
@@ -4992,15 +5304,19 @@
         <v>1600</v>
       </c>
       <c r="L73" t="n">
-        <v>700</v>
-      </c>
-      <c r="M73" t="inlineStr"/>
-      <c r="N73" t="inlineStr"/>
+        <v>545</v>
+      </c>
+      <c r="M73" t="n">
+        <v>460</v>
+      </c>
+      <c r="N73" t="n">
+        <v>545</v>
+      </c>
       <c r="O73" t="n">
-        <v>700</v>
+        <v>545</v>
       </c>
       <c r="P73" t="n">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="Q73" t="n">
         <v>30</v>
@@ -5013,7 +5329,9 @@
           <t>ok</t>
         </is>
       </c>
-      <c r="T73" t="inlineStr"/>
+      <c r="T73" t="n">
+        <v>0.18</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -5167,7 +5485,9 @@
       <c r="G76" t="n">
         <v>860</v>
       </c>
-      <c r="H76" t="inlineStr"/>
+      <c r="H76" t="n">
+        <v>800</v>
+      </c>
       <c r="I76" t="n">
         <v>890</v>
       </c>
@@ -5178,15 +5498,19 @@
         <v>1600</v>
       </c>
       <c r="L76" t="n">
-        <v>650</v>
-      </c>
-      <c r="M76" t="inlineStr"/>
-      <c r="N76" t="inlineStr"/>
+        <v>545</v>
+      </c>
+      <c r="M76" t="n">
+        <v>460</v>
+      </c>
+      <c r="N76" t="n">
+        <v>545</v>
+      </c>
       <c r="O76" t="n">
-        <v>650</v>
+        <v>545</v>
       </c>
       <c r="P76" t="n">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="Q76" t="n">
         <v>36.36363636363637</v>
@@ -5199,7 +5523,9 @@
           <t>ok</t>
         </is>
       </c>
-      <c r="T76" t="inlineStr"/>
+      <c r="T76" t="n">
+        <v>0.18</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -5227,28 +5553,34 @@
         </is>
       </c>
       <c r="G77" t="n">
-        <v>880</v>
-      </c>
-      <c r="H77" t="inlineStr"/>
+        <v>870</v>
+      </c>
+      <c r="H77" t="n">
+        <v>800</v>
+      </c>
       <c r="I77" t="n">
-        <v>900</v>
+        <v>930</v>
       </c>
       <c r="J77" t="n">
         <v>0.18</v>
       </c>
       <c r="K77" t="n">
-        <v>1500</v>
+        <v>1300</v>
       </c>
       <c r="L77" t="n">
-        <v>655</v>
-      </c>
-      <c r="M77" t="inlineStr"/>
-      <c r="N77" t="inlineStr"/>
+        <v>570</v>
+      </c>
+      <c r="M77" t="n">
+        <v>480</v>
+      </c>
+      <c r="N77" t="n">
+        <v>570</v>
+      </c>
       <c r="O77" t="n">
-        <v>655</v>
+        <v>570</v>
       </c>
       <c r="P77" t="n">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="Q77" t="n">
         <v>34.95145631067961</v>
@@ -5261,7 +5593,9 @@
           <t>ok</t>
         </is>
       </c>
-      <c r="T77" t="inlineStr"/>
+      <c r="T77" t="n">
+        <v>0.18</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -5537,11 +5871,13 @@
         </is>
       </c>
       <c r="G82" t="n">
-        <v>860</v>
-      </c>
-      <c r="H82" t="inlineStr"/>
+        <v>880</v>
+      </c>
+      <c r="H82" t="n">
+        <v>800</v>
+      </c>
       <c r="I82" t="n">
-        <v>910</v>
+        <v>930</v>
       </c>
       <c r="J82" t="n">
         <v>0.16</v>
@@ -5550,15 +5886,19 @@
         <v>1600</v>
       </c>
       <c r="L82" t="n">
-        <v>680</v>
-      </c>
-      <c r="M82" t="inlineStr"/>
-      <c r="N82" t="inlineStr"/>
+        <v>530</v>
+      </c>
+      <c r="M82" t="n">
+        <v>460</v>
+      </c>
+      <c r="N82" t="n">
+        <v>530</v>
+      </c>
       <c r="O82" t="n">
-        <v>680</v>
+        <v>530</v>
       </c>
       <c r="P82" t="n">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="Q82" t="n">
         <v>30</v>
@@ -5571,7 +5911,9 @@
           <t>ok</t>
         </is>
       </c>
-      <c r="T82" t="inlineStr"/>
+      <c r="T82" t="n">
+        <v>0.16</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -5661,11 +6003,13 @@
         </is>
       </c>
       <c r="G84" t="n">
-        <v>870</v>
-      </c>
-      <c r="H84" t="inlineStr"/>
+        <v>880</v>
+      </c>
+      <c r="H84" t="n">
+        <v>800</v>
+      </c>
       <c r="I84" t="n">
-        <v>900</v>
+        <v>930</v>
       </c>
       <c r="J84" t="n">
         <v>0.16</v>
@@ -5674,15 +6018,19 @@
         <v>1600</v>
       </c>
       <c r="L84" t="n">
-        <v>690</v>
-      </c>
-      <c r="M84" t="inlineStr"/>
-      <c r="N84" t="inlineStr"/>
+        <v>530</v>
+      </c>
+      <c r="M84" t="n">
+        <v>460</v>
+      </c>
+      <c r="N84" t="n">
+        <v>530</v>
+      </c>
       <c r="O84" t="n">
-        <v>690</v>
+        <v>530</v>
       </c>
       <c r="P84" t="n">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="Q84" t="n">
         <v>31.30434782608696</v>
@@ -5695,7 +6043,9 @@
           <t>ok</t>
         </is>
       </c>
-      <c r="T84" t="inlineStr"/>
+      <c r="T84" t="n">
+        <v>0.16</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -5723,11 +6073,13 @@
         </is>
       </c>
       <c r="G85" t="n">
-        <v>870</v>
-      </c>
-      <c r="H85" t="inlineStr"/>
+        <v>880</v>
+      </c>
+      <c r="H85" t="n">
+        <v>800</v>
+      </c>
       <c r="I85" t="n">
-        <v>890</v>
+        <v>930</v>
       </c>
       <c r="J85" t="n">
         <v>0.16</v>
@@ -5736,15 +6088,19 @@
         <v>1600</v>
       </c>
       <c r="L85" t="n">
-        <v>680</v>
-      </c>
-      <c r="M85" t="inlineStr"/>
-      <c r="N85" t="inlineStr"/>
+        <v>530</v>
+      </c>
+      <c r="M85" t="n">
+        <v>460</v>
+      </c>
+      <c r="N85" t="n">
+        <v>530</v>
+      </c>
       <c r="O85" t="n">
-        <v>680</v>
+        <v>530</v>
       </c>
       <c r="P85" t="n">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="Q85" t="n">
         <v>31.30434782608696</v>
@@ -5757,7 +6113,9 @@
           <t>ok</t>
         </is>
       </c>
-      <c r="T85" t="inlineStr"/>
+      <c r="T85" t="n">
+        <v>0.16</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -5971,28 +6329,34 @@
         </is>
       </c>
       <c r="G89" t="n">
-        <v>880</v>
-      </c>
-      <c r="H89" t="inlineStr"/>
+        <v>860</v>
+      </c>
+      <c r="H89" t="n">
+        <v>800</v>
+      </c>
       <c r="I89" t="n">
-        <v>930</v>
+        <v>890</v>
       </c>
       <c r="J89" t="n">
         <v>0.14</v>
       </c>
       <c r="K89" t="n">
-        <v>1550</v>
+        <v>1600</v>
       </c>
       <c r="L89" t="n">
-        <v>635</v>
-      </c>
-      <c r="M89" t="inlineStr"/>
-      <c r="N89" t="inlineStr"/>
+        <v>596</v>
+      </c>
+      <c r="M89" t="n">
+        <v>450</v>
+      </c>
+      <c r="N89" t="n">
+        <v>596</v>
+      </c>
       <c r="O89" t="n">
-        <v>635</v>
+        <v>596</v>
       </c>
       <c r="P89" t="n">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="Q89" t="n">
         <v>28.8</v>
@@ -6005,7 +6369,9 @@
           <t>ok</t>
         </is>
       </c>
-      <c r="T89" t="inlineStr"/>
+      <c r="T89" t="n">
+        <v>0.15</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -6035,7 +6401,9 @@
       <c r="G90" t="n">
         <v>860</v>
       </c>
-      <c r="H90" t="inlineStr"/>
+      <c r="H90" t="n">
+        <v>800</v>
+      </c>
       <c r="I90" t="n">
         <v>890</v>
       </c>
@@ -6046,12 +6414,16 @@
         <v>1600</v>
       </c>
       <c r="L90" t="n">
-        <v>595</v>
-      </c>
-      <c r="M90" t="inlineStr"/>
-      <c r="N90" t="inlineStr"/>
+        <v>596</v>
+      </c>
+      <c r="M90" t="n">
+        <v>450</v>
+      </c>
+      <c r="N90" t="n">
+        <v>596</v>
+      </c>
       <c r="O90" t="n">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="P90" t="n">
         <v>115</v>
@@ -6067,7 +6439,9 @@
           <t>ok</t>
         </is>
       </c>
-      <c r="T90" t="inlineStr"/>
+      <c r="T90" t="n">
+        <v>0.15</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -6157,9 +6531,11 @@
         </is>
       </c>
       <c r="G92" t="n">
-        <v>860</v>
-      </c>
-      <c r="H92" t="inlineStr"/>
+        <v>880</v>
+      </c>
+      <c r="H92" t="n">
+        <v>800</v>
+      </c>
       <c r="I92" t="n">
         <v>920</v>
       </c>
@@ -6170,12 +6546,16 @@
         <v>1600</v>
       </c>
       <c r="L92" t="n">
-        <v>570</v>
-      </c>
-      <c r="M92" t="inlineStr"/>
-      <c r="N92" t="inlineStr"/>
+        <v>572</v>
+      </c>
+      <c r="M92" t="n">
+        <v>500</v>
+      </c>
+      <c r="N92" t="n">
+        <v>572</v>
+      </c>
       <c r="O92" t="n">
-        <v>570</v>
+        <v>572</v>
       </c>
       <c r="P92" t="n">
         <v>110</v>
@@ -6191,7 +6571,9 @@
           <t>ok</t>
         </is>
       </c>
-      <c r="T92" t="inlineStr"/>
+      <c r="T92" t="n">
+        <v>0.18</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -6345,25 +6727,31 @@
         </is>
       </c>
       <c r="G95" t="n">
-        <v>830</v>
-      </c>
-      <c r="H95" t="inlineStr"/>
+        <v>820</v>
+      </c>
+      <c r="H95" t="n">
+        <v>800</v>
+      </c>
       <c r="I95" t="n">
-        <v>910</v>
+        <v>920</v>
       </c>
       <c r="J95" t="n">
         <v>0.37</v>
       </c>
       <c r="K95" t="n">
-        <v>1250</v>
+        <v>1400</v>
       </c>
       <c r="L95" t="n">
         <v>600</v>
       </c>
-      <c r="M95" t="inlineStr"/>
-      <c r="N95" t="inlineStr"/>
+      <c r="M95" t="n">
+        <v>590</v>
+      </c>
+      <c r="N95" t="n">
+        <v>707</v>
+      </c>
       <c r="O95" t="n">
-        <v>705</v>
+        <v>707</v>
       </c>
       <c r="P95" t="n">
         <v>60</v>
@@ -6379,7 +6767,9 @@
           <t>ok</t>
         </is>
       </c>
-      <c r="T95" t="inlineStr"/>
+      <c r="T95" t="n">
+        <v>0.35</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -6469,25 +6859,31 @@
         </is>
       </c>
       <c r="G97" t="n">
-        <v>830</v>
-      </c>
-      <c r="H97" t="inlineStr"/>
+        <v>820</v>
+      </c>
+      <c r="H97" t="n">
+        <v>800</v>
+      </c>
       <c r="I97" t="n">
-        <v>910</v>
+        <v>940</v>
       </c>
       <c r="J97" t="n">
         <v>0.37</v>
       </c>
       <c r="K97" t="n">
-        <v>1250</v>
+        <v>1350</v>
       </c>
       <c r="L97" t="n">
         <v>610</v>
       </c>
-      <c r="M97" t="inlineStr"/>
-      <c r="N97" t="inlineStr"/>
+      <c r="M97" t="n">
+        <v>560</v>
+      </c>
+      <c r="N97" t="n">
+        <v>650</v>
+      </c>
       <c r="O97" t="n">
-        <v>655</v>
+        <v>650</v>
       </c>
       <c r="P97" t="n">
         <v>48</v>
@@ -6503,7 +6899,9 @@
           <t>ok</t>
         </is>
       </c>
-      <c r="T97" t="inlineStr"/>
+      <c r="T97" t="n">
+        <v>0.34</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -6965,28 +7363,34 @@
         </is>
       </c>
       <c r="G105" t="n">
-        <v>830</v>
-      </c>
-      <c r="H105" t="inlineStr"/>
+        <v>860</v>
+      </c>
+      <c r="H105" t="n">
+        <v>800</v>
+      </c>
       <c r="I105" t="n">
-        <v>910</v>
+        <v>940</v>
       </c>
       <c r="J105" t="n">
         <v>0.35</v>
       </c>
       <c r="K105" t="n">
-        <v>1350</v>
+        <v>1400</v>
       </c>
       <c r="L105" t="n">
-        <v>525</v>
-      </c>
-      <c r="M105" t="inlineStr"/>
-      <c r="N105" t="inlineStr"/>
+        <v>655</v>
+      </c>
+      <c r="M105" t="n">
+        <v>560</v>
+      </c>
+      <c r="N105" t="n">
+        <v>655</v>
+      </c>
       <c r="O105" t="n">
-        <v>525</v>
+        <v>655</v>
       </c>
       <c r="P105" t="n">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="Q105" t="n">
         <v>70.58823529411765</v>
@@ -6999,7 +7403,9 @@
           <t>ok</t>
         </is>
       </c>
-      <c r="T105" t="inlineStr"/>
+      <c r="T105" t="n">
+        <v>0.34</v>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -7525,9 +7931,11 @@
         </is>
       </c>
       <c r="G114" t="n">
-        <v>840</v>
-      </c>
-      <c r="H114" t="inlineStr"/>
+        <v>880</v>
+      </c>
+      <c r="H114" t="n">
+        <v>800</v>
+      </c>
       <c r="I114" t="n">
         <v>910</v>
       </c>
@@ -7538,15 +7946,19 @@
         <v>1400</v>
       </c>
       <c r="L114" t="n">
-        <v>695</v>
-      </c>
-      <c r="M114" t="inlineStr"/>
-      <c r="N114" t="inlineStr"/>
+        <v>660</v>
+      </c>
+      <c r="M114" t="n">
+        <v>560</v>
+      </c>
+      <c r="N114" t="n">
+        <v>660</v>
+      </c>
       <c r="O114" t="n">
-        <v>695</v>
+        <v>660</v>
       </c>
       <c r="P114" t="n">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="Q114" t="n">
         <v>70.58823529411765</v>
@@ -7559,7 +7971,9 @@
           <t>ok</t>
         </is>
       </c>
-      <c r="T114" t="inlineStr"/>
+      <c r="T114" t="n">
+        <v>0.33</v>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">

</xml_diff>